<commit_message>
added the values to the excel table
</commit_message>
<xml_diff>
--- a/AI-Assignment-3/Book1.xlsx
+++ b/AI-Assignment-3/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkhal\Documents\GitHub\ai-assignments\AI-Assignment-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4th sem\ai\ai-assignments\AI-Assignment-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410047A0-437E-41AF-93AB-112D6770CFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231FF4A6-F7F9-4F91-94E1-F4D7AB8B9B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{90D19855-AE84-4057-B551-F8241F3138E8}"/>
+    <workbookView xWindow="12240" yWindow="1440" windowWidth="15375" windowHeight="7875" xr2:uid="{90D19855-AE84-4057-B551-F8241F3138E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -269,7 +269,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -300,6 +300,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
@@ -621,33 +623,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F807ACDE-BC40-4A2F-9BDC-3E8EAFF35EE9}">
-  <dimension ref="C4:P42"/>
+  <dimension ref="C4:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
@@ -667,7 +669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -677,7 +679,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="7">
         <v>1</v>
       </c>
@@ -697,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="7">
         <v>2</v>
       </c>
@@ -717,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="7">
         <v>3</v>
       </c>
@@ -737,7 +739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="7">
         <v>4</v>
       </c>
@@ -757,7 +759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="3">
         <v>1</v>
       </c>
@@ -777,7 +779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="3">
         <v>2</v>
       </c>
@@ -797,7 +799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="3">
         <v>3</v>
       </c>
@@ -817,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="3">
         <v>4</v>
       </c>
@@ -837,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="7">
         <v>1</v>
       </c>
@@ -857,7 +859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="7">
         <v>2</v>
       </c>
@@ -877,7 +879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="7">
         <v>3</v>
       </c>
@@ -897,7 +899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="7">
         <v>4</v>
       </c>
@@ -917,8 +919,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="3:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
@@ -953,7 +955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="3:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -968,7 +970,7 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C31" s="3">
         <v>4</v>
       </c>
@@ -1005,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C32" s="3">
         <v>6</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C33" s="3">
         <v>8</v>
       </c>
@@ -1075,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C34" s="3">
         <v>10</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C35" s="3">
         <v>15</v>
       </c>
@@ -1145,7 +1147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C36" s="3">
         <v>20</v>
       </c>
@@ -1180,7 +1182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C37" s="3">
         <v>25</v>
       </c>
@@ -1212,7 +1214,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C40" s="13" t="s">
         <v>18</v>
       </c>
@@ -1253,7 +1255,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C42" s="11" t="s">
         <v>16</v>
       </c>
@@ -1291,8 +1293,256 @@
         <v>24</v>
       </c>
     </row>
+    <row r="43" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>4</v>
+      </c>
+      <c r="J43">
+        <v>7</v>
+      </c>
+      <c r="K43">
+        <v>11</v>
+      </c>
+      <c r="L43">
+        <v>16</v>
+      </c>
+      <c r="M43">
+        <v>3</v>
+      </c>
+      <c r="N43">
+        <v>6</v>
+      </c>
+      <c r="O43">
+        <v>6</v>
+      </c>
+      <c r="P43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>6</v>
+      </c>
+      <c r="E44">
+        <v>10</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>4</v>
+      </c>
+      <c r="J44">
+        <v>3</v>
+      </c>
+      <c r="K44">
+        <v>4</v>
+      </c>
+      <c r="L44">
+        <v>5</v>
+      </c>
+      <c r="M44">
+        <v>5</v>
+      </c>
+      <c r="N44">
+        <v>5</v>
+      </c>
+      <c r="O44">
+        <v>5</v>
+      </c>
+      <c r="P44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <v>25</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="I45" s="14">
+        <v>8</v>
+      </c>
+      <c r="J45">
+        <v>15</v>
+      </c>
+      <c r="K45">
+        <v>25</v>
+      </c>
+      <c r="L45">
+        <v>38</v>
+      </c>
+      <c r="M45">
+        <v>5</v>
+      </c>
+      <c r="N45">
+        <v>5</v>
+      </c>
+      <c r="O45">
+        <v>5</v>
+      </c>
+      <c r="P45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="E46">
+        <v>50</v>
+      </c>
+      <c r="G46" s="14">
+        <v>17</v>
+      </c>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14">
+        <v>21</v>
+      </c>
+      <c r="J46" s="14">
+        <v>25</v>
+      </c>
+      <c r="K46" s="14">
+        <v>29</v>
+      </c>
+      <c r="L46" s="14">
+        <v>34</v>
+      </c>
+      <c r="M46" s="14">
+        <v>8</v>
+      </c>
+      <c r="N46" s="14">
+        <v>18</v>
+      </c>
+      <c r="O46" s="14">
+        <v>22</v>
+      </c>
+      <c r="P46" s="14">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>15</v>
+      </c>
+      <c r="E47">
+        <v>150</v>
+      </c>
+      <c r="G47" s="14">
+        <v>26</v>
+      </c>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14">
+        <v>31</v>
+      </c>
+      <c r="J47" s="14">
+        <v>42</v>
+      </c>
+      <c r="K47" s="14">
+        <v>58</v>
+      </c>
+      <c r="L47" s="14">
+        <v>79</v>
+      </c>
+      <c r="M47" s="14">
+        <v>23</v>
+      </c>
+      <c r="N47" s="14">
+        <v>29</v>
+      </c>
+      <c r="O47" s="14">
+        <v>80</v>
+      </c>
+      <c r="P47" s="14">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>20</v>
+      </c>
+      <c r="E48">
+        <v>75</v>
+      </c>
+      <c r="G48" s="14">
+        <v>15</v>
+      </c>
+      <c r="I48" s="14">
+        <v>22</v>
+      </c>
+      <c r="J48" s="14">
+        <v>35</v>
+      </c>
+      <c r="K48" s="14">
+        <v>54</v>
+      </c>
+      <c r="L48" s="14">
+        <v>79</v>
+      </c>
+      <c r="M48" s="14">
+        <v>13</v>
+      </c>
+      <c r="N48" s="14">
+        <v>24</v>
+      </c>
+      <c r="O48" s="15">
+        <v>34</v>
+      </c>
+      <c r="P48" s="15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>25</v>
+      </c>
+      <c r="E49">
+        <v>100</v>
+      </c>
+      <c r="G49" s="15">
+        <v>20</v>
+      </c>
+      <c r="I49" s="14">
+        <v>25</v>
+      </c>
+      <c r="J49" s="14">
+        <v>34</v>
+      </c>
+      <c r="K49" s="14">
+        <v>47</v>
+      </c>
+      <c r="L49" s="14">
+        <v>64</v>
+      </c>
+      <c r="M49" s="14">
+        <v>8</v>
+      </c>
+      <c r="N49" s="14">
+        <v>11</v>
+      </c>
+      <c r="O49" s="14">
+        <v>15</v>
+      </c>
+      <c r="P49" s="15">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Stages of report
</commit_message>
<xml_diff>
--- a/AI-Assignment-3/Book1.xlsx
+++ b/AI-Assignment-3/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4th sem\ai\ai-assignments\AI-Assignment-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkhal\Documents\GitHub\ai-assignments\AI-Assignment-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231FF4A6-F7F9-4F91-94E1-F4D7AB8B9B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429D603B-FC3F-42D8-8E6D-3D8B2254762C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="1440" windowWidth="15375" windowHeight="7875" xr2:uid="{90D19855-AE84-4057-B551-F8241F3138E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{90D19855-AE84-4057-B551-F8241F3138E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="32">
   <si>
     <t>No of vars</t>
   </si>
@@ -110,6 +110,24 @@
   </si>
   <si>
     <t>Beam Width 4</t>
+  </si>
+  <si>
+    <t>No. of Variables</t>
+  </si>
+  <si>
+    <t>No. of Clause</t>
+  </si>
+  <si>
+    <t>States explored</t>
+  </si>
+  <si>
+    <t>Reached</t>
+  </si>
+  <si>
+    <t>Not Reached</t>
+  </si>
+  <si>
+    <t>VND</t>
   </si>
 </sst>
 </file>
@@ -175,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +237,18 @@
         <fgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -259,7 +289,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -268,8 +298,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,9 +334,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
+    <cellStyle name="40% - Accent1" xfId="8" builtinId="31"/>
+    <cellStyle name="60% - Accent4" xfId="9" builtinId="44"/>
     <cellStyle name="60% - Accent6" xfId="6" builtinId="52"/>
     <cellStyle name="Accent1" xfId="7" builtinId="29"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -623,33 +659,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F807ACDE-BC40-4A2F-9BDC-3E8EAFF35EE9}">
-  <dimension ref="C4:P49"/>
+  <dimension ref="C4:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O50" sqref="O50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.88671875" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.77734375" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" customWidth="1"/>
+    <col min="19" max="19" width="14.44140625" customWidth="1"/>
+    <col min="20" max="20" width="15.21875" customWidth="1"/>
+    <col min="21" max="21" width="11.5546875" customWidth="1"/>
+    <col min="22" max="22" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
@@ -669,7 +710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="3"/>
@@ -679,7 +720,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C6" s="7">
         <v>1</v>
       </c>
@@ -699,7 +740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C7" s="7">
         <v>2</v>
       </c>
@@ -719,7 +760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" s="7">
         <v>3</v>
       </c>
@@ -739,7 +780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="7">
         <v>4</v>
       </c>
@@ -759,7 +800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>1</v>
       </c>
@@ -779,7 +820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>2</v>
       </c>
@@ -799,7 +840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>3</v>
       </c>
@@ -819,7 +860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>4</v>
       </c>
@@ -839,7 +880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" s="7">
         <v>1</v>
       </c>
@@ -859,7 +900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C15" s="7">
         <v>2</v>
       </c>
@@ -879,7 +920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" s="7">
         <v>3</v>
       </c>
@@ -899,7 +940,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C17" s="7">
         <v>4</v>
       </c>
@@ -919,8 +960,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="3:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="3:15" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
@@ -955,7 +996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -970,7 +1011,7 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
     </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C31" s="3">
         <v>4</v>
       </c>
@@ -1007,7 +1048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>6</v>
       </c>
@@ -1042,7 +1083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C33" s="3">
         <v>8</v>
       </c>
@@ -1077,7 +1118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C34" s="3">
         <v>10</v>
       </c>
@@ -1112,7 +1153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C35" s="3">
         <v>15</v>
       </c>
@@ -1147,7 +1188,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C36" s="3">
         <v>20</v>
       </c>
@@ -1182,7 +1223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C37" s="3">
         <v>25</v>
       </c>
@@ -1214,7 +1255,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C40" s="13" t="s">
         <v>18</v>
       </c>
@@ -1255,7 +1296,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C42" s="11" t="s">
         <v>16</v>
       </c>
@@ -1265,7 +1306,7 @@
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="11" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="11" t="s">
@@ -1293,116 +1334,116 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C43">
-        <v>4</v>
-      </c>
-      <c r="E43">
-        <v>5</v>
-      </c>
-      <c r="G43">
-        <v>2</v>
-      </c>
-      <c r="I43">
-        <v>4</v>
-      </c>
-      <c r="J43">
+    <row r="43" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C43" s="16">
+        <v>4</v>
+      </c>
+      <c r="E43" s="16">
+        <v>5</v>
+      </c>
+      <c r="G43" s="15">
+        <v>2</v>
+      </c>
+      <c r="I43" s="15">
+        <v>4</v>
+      </c>
+      <c r="J43" s="15">
         <v>7</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="15">
         <v>11</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="15">
         <v>16</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="15">
         <v>3</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="15">
         <v>6</v>
       </c>
-      <c r="O43">
+      <c r="O43" s="15">
         <v>6</v>
       </c>
-      <c r="P43">
+      <c r="P43" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C44">
+    <row r="44" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C44" s="16">
         <v>6</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="16">
         <v>10</v>
       </c>
-      <c r="G44">
-        <v>2</v>
-      </c>
-      <c r="I44">
-        <v>4</v>
-      </c>
-      <c r="J44">
+      <c r="G44" s="15">
+        <v>2</v>
+      </c>
+      <c r="I44" s="15">
+        <v>4</v>
+      </c>
+      <c r="J44" s="15">
         <v>3</v>
       </c>
-      <c r="K44">
-        <v>4</v>
-      </c>
-      <c r="L44">
-        <v>5</v>
-      </c>
-      <c r="M44">
-        <v>5</v>
-      </c>
-      <c r="N44">
-        <v>5</v>
-      </c>
-      <c r="O44">
-        <v>5</v>
-      </c>
-      <c r="P44">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C45">
+      <c r="K44" s="15">
+        <v>4</v>
+      </c>
+      <c r="L44" s="15">
+        <v>5</v>
+      </c>
+      <c r="M44" s="15">
+        <v>5</v>
+      </c>
+      <c r="N44" s="15">
+        <v>5</v>
+      </c>
+      <c r="O44" s="15">
+        <v>5</v>
+      </c>
+      <c r="P44" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C45" s="16">
         <v>8</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="16">
         <v>25</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="15">
         <v>4</v>
       </c>
       <c r="I45" s="14">
         <v>8</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="15">
         <v>15</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="15">
         <v>25</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="15">
         <v>38</v>
       </c>
-      <c r="M45">
-        <v>5</v>
-      </c>
-      <c r="N45">
-        <v>5</v>
-      </c>
-      <c r="O45">
-        <v>5</v>
-      </c>
-      <c r="P45">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C46">
+      <c r="M45" s="15">
+        <v>5</v>
+      </c>
+      <c r="N45" s="15">
+        <v>5</v>
+      </c>
+      <c r="O45" s="15">
+        <v>5</v>
+      </c>
+      <c r="P45" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C46" s="16">
         <v>10</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="16">
         <v>50</v>
       </c>
       <c r="G46" s="14">
@@ -1434,11 +1475,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C47">
+    <row r="47" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C47" s="16">
         <v>15</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="16">
         <v>150</v>
       </c>
       <c r="G47" s="14">
@@ -1470,11 +1511,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C48">
+    <row r="48" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="C48" s="16">
         <v>20</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="16">
         <v>75</v>
       </c>
       <c r="G48" s="14">
@@ -1505,11 +1546,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C49">
+    <row r="49" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C49" s="16">
         <v>25</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="16">
         <v>100</v>
       </c>
       <c r="G49" s="15">
@@ -1538,6 +1579,244 @@
       </c>
       <c r="P49" s="15">
         <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R51" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="S51" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="T51" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="U51" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="V51" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R53" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="S53" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="T53" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="U53" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="V53" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <v>4</v>
+      </c>
+      <c r="T54">
+        <v>5</v>
+      </c>
+      <c r="U54" t="s">
+        <v>29</v>
+      </c>
+      <c r="V54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R55">
+        <v>2</v>
+      </c>
+      <c r="S55">
+        <v>4</v>
+      </c>
+      <c r="T55">
+        <v>5</v>
+      </c>
+      <c r="U55" t="s">
+        <v>29</v>
+      </c>
+      <c r="V55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R56">
+        <v>3</v>
+      </c>
+      <c r="S56">
+        <v>4</v>
+      </c>
+      <c r="T56">
+        <v>5</v>
+      </c>
+      <c r="U56" t="s">
+        <v>29</v>
+      </c>
+      <c r="V56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R57">
+        <v>4</v>
+      </c>
+      <c r="S57">
+        <v>4</v>
+      </c>
+      <c r="T57">
+        <v>5</v>
+      </c>
+      <c r="U57" t="s">
+        <v>29</v>
+      </c>
+      <c r="V57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R58">
+        <v>1</v>
+      </c>
+      <c r="S58">
+        <v>10</v>
+      </c>
+      <c r="T58">
+        <v>50</v>
+      </c>
+      <c r="U58" t="s">
+        <v>30</v>
+      </c>
+      <c r="V58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R59">
+        <v>2</v>
+      </c>
+      <c r="S59">
+        <v>10</v>
+      </c>
+      <c r="T59">
+        <v>50</v>
+      </c>
+      <c r="U59" t="s">
+        <v>30</v>
+      </c>
+      <c r="V59">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R60">
+        <v>3</v>
+      </c>
+      <c r="S60">
+        <v>10</v>
+      </c>
+      <c r="T60">
+        <v>50</v>
+      </c>
+      <c r="U60" t="s">
+        <v>30</v>
+      </c>
+      <c r="V60">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R61">
+        <v>4</v>
+      </c>
+      <c r="S61">
+        <v>10</v>
+      </c>
+      <c r="T61">
+        <v>50</v>
+      </c>
+      <c r="U61" t="s">
+        <v>30</v>
+      </c>
+      <c r="V61">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <v>20</v>
+      </c>
+      <c r="T62">
+        <v>75</v>
+      </c>
+      <c r="U62" t="s">
+        <v>30</v>
+      </c>
+      <c r="V62">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R63">
+        <v>2</v>
+      </c>
+      <c r="S63">
+        <v>20</v>
+      </c>
+      <c r="T63">
+        <v>75</v>
+      </c>
+      <c r="U63" t="s">
+        <v>30</v>
+      </c>
+      <c r="V63">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="R64">
+        <v>3</v>
+      </c>
+      <c r="S64">
+        <v>20</v>
+      </c>
+      <c r="T64">
+        <v>75</v>
+      </c>
+      <c r="U64" t="s">
+        <v>29</v>
+      </c>
+      <c r="V64">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R65">
+        <v>4</v>
+      </c>
+      <c r="S65">
+        <v>20</v>
+      </c>
+      <c r="T65">
+        <v>75</v>
+      </c>
+      <c r="U65" t="s">
+        <v>29</v>
+      </c>
+      <c r="V65">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>